<commit_message>
add bt-buoi-04 Sáng t2 22/06
</commit_message>
<xml_diff>
--- a/PHP-Course/BackEnd-PHP/Ch-02-ASNT/Array.xlsx
+++ b/PHP-Course/BackEnd-PHP/Ch-02-ASNT/Array.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ASNT" sheetId="13" r:id="rId1"/>
@@ -1393,29 +1393,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1438,6 +1420,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1941,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,7 +2414,7 @@
       <c r="H36" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I36" s="43" t="s">
+      <c r="I36" s="57" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       <c r="H37" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="I37" s="44"/>
+      <c r="I37" s="58"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
@@ -2450,7 +2450,7 @@
       <c r="H38" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="I38" s="44"/>
+      <c r="I38" s="58"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G39" s="25"/>
@@ -2468,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2906,7 +2906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
@@ -3683,8 +3683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P78" sqref="P78"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="O53" sqref="O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4009,10 +4009,10 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="45"/>
+      <c r="D28" s="59"/>
       <c r="E28" s="9"/>
       <c r="F28" s="10"/>
       <c r="I28" s="12" t="s">
@@ -4069,7 +4069,7 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="45"/>
+      <c r="D29" s="59"/>
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
       <c r="I29" s="12" t="s">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
-      <c r="D30" s="46"/>
+      <c r="D30" s="60"/>
       <c r="E30" s="14"/>
       <c r="F30" s="15"/>
       <c r="I30" s="38" t="s">
@@ -4671,7 +4671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
@@ -6024,7 +6024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
@@ -6142,47 +6142,47 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="51" t="s">
+      <c r="G6" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="49" t="s">
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="L6" s="57" t="s">
+      <c r="L6" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="53"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="47"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="54" t="s">
+      <c r="F7" s="62"/>
+      <c r="G7" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="58" t="s">
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="52" t="s">
         <v>51</v>
       </c>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="59"/>
+      <c r="P7" s="53"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -6198,13 +6198,13 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="58" t="s">
+      <c r="L8" s="52" t="s">
         <v>226</v>
       </c>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
-      <c r="P8" s="59"/>
+      <c r="P8" s="53"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
@@ -6220,13 +6220,13 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="58" t="s">
+      <c r="L9" s="52" t="s">
         <v>227</v>
       </c>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
-      <c r="P9" s="59"/>
+      <c r="P9" s="53"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -6242,11 +6242,11 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="60"/>
+      <c r="L10" s="54"/>
       <c r="M10" s="16"/>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="59"/>
+      <c r="P10" s="53"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -6262,13 +6262,13 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="52" t="s">
         <v>55</v>
       </c>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="59"/>
+      <c r="P11" s="53"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -6288,7 +6288,7 @@
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
-      <c r="P12" s="59"/>
+      <c r="P12" s="53"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -6304,13 +6304,13 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="58" t="s">
+      <c r="L13" s="52" t="s">
         <v>50</v>
       </c>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
-      <c r="P13" s="59"/>
+      <c r="P13" s="53"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -6326,13 +6326,13 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="58" t="s">
+      <c r="L14" s="52" t="s">
         <v>51</v>
       </c>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="59"/>
+      <c r="P14" s="53"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -6348,13 +6348,13 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
-      <c r="L15" s="58" t="s">
+      <c r="L15" s="52" t="s">
         <v>228</v>
       </c>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
-      <c r="P15" s="59"/>
+      <c r="P15" s="53"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
@@ -6368,13 +6368,13 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="61" t="s">
+      <c r="L16" s="55" t="s">
         <v>229</v>
       </c>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="56"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="50"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
@@ -6474,7 +6474,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="10"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="48"/>
+      <c r="J22" s="44"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
@@ -6516,7 +6516,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="10"/>
       <c r="I24" s="9"/>
-      <c r="J24" s="48"/>
+      <c r="J24" s="44"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
@@ -6556,7 +6556,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="10"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="48"/>
+      <c r="J26" s="44"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
@@ -6597,10 +6597,10 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="49" t="s">
+      <c r="I28" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="J28" s="48"/>
+      <c r="J28" s="44"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
@@ -6619,7 +6619,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="50"/>
+      <c r="I29" s="62"/>
       <c r="J29" s="22" t="s">
         <v>237</v>
       </c>
@@ -6642,7 +6642,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="10"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="48"/>
+      <c r="J30" s="44"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
@@ -6682,7 +6682,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="10"/>
       <c r="I32" s="9"/>
-      <c r="J32" s="48"/>
+      <c r="J32" s="44"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
@@ -6724,7 +6724,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="10"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="48"/>
+      <c r="J34" s="44"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
@@ -6773,7 +6773,7 @@
       <c r="P36" s="15"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J37" s="47"/>
+      <c r="J37" s="43"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -6882,7 +6882,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="10"/>
-      <c r="J43" s="48"/>
+      <c r="J43" s="44"/>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
@@ -6924,7 +6924,7 @@
       <c r="G45" s="9"/>
       <c r="H45" s="10"/>
       <c r="I45" s="64"/>
-      <c r="J45" s="48"/>
+      <c r="J45" s="44"/>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
@@ -7002,7 +7002,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="10"/>
-      <c r="J49" s="48"/>
+      <c r="J49" s="44"/>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
@@ -7068,7 +7068,7 @@
       <c r="O52" s="15"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J53" s="47"/>
+      <c r="J53" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>